<commit_message>
Inclusão do pacote Power BI
Inclusão dos arquivos que trazer o codigo fonte
</commit_message>
<xml_diff>
--- a/Wolrd Population Data.xlsx
+++ b/Wolrd Population Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263d74c401730189/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263d74c401730189/Desktop/Wold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{7AC64A1E-81AA-459C-B91C-A743A76CC10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74DF9BC5-C592-450D-BCA0-3E11780018F8}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{7AC64A1E-81AA-459C-B91C-A743A76CC10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0038BDB3-9593-4042-8CE1-0D6D65EE391B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A9A4517-54CC-463D-B5FC-53C5F03393D4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
   <si>
     <t>Rank</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Venezuela</t>
-  </si>
-  <si>
-    <t>N.A.</t>
   </si>
   <si>
     <t>Niger</t>
@@ -782,7 +779,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1282,7 +1279,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1332,7 +1329,13 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0_ ;[Red]\-0\ "/>
@@ -1343,17 +1346,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1386,14 +1383,14 @@
     <tableColumn id="2" xr3:uid="{A7480106-A65C-48C7-84E9-060389FC7134}" name="Country" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{4EC52585-D6F6-4D64-B4E4-399D26A08785}" name="Population (2024)" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{F0290345-2A39-431A-8F0F-7B2DFC7127B0}" name="Mudanca_Anual" dataCellStyle="Porcentagem"/>
-    <tableColumn id="5" xr3:uid="{4CC63AA6-A78C-42B8-85A4-140D8A90862B}" name="Mudanca_Liquida" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F48D8035-F4B0-4B4D-8A5A-AEA88F7EFD59}" name="Density (P/KmÂ²)" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{4BA3AD05-1A6C-40E6-8D5A-7BDE9743BF2B}" name=" Area (KmÂ²)" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0E49A9D5-D603-4E94-A8D7-A4BB044C0D68}" name="Migrants (net)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{3870A96F-5DEC-436D-B51A-9A68E50275AD}" name="Fert. Rate" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{4CC63AA6-A78C-42B8-85A4-140D8A90862B}" name="Mudanca_Liquida" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F48D8035-F4B0-4B4D-8A5A-AEA88F7EFD59}" name="Density (P/KmÂ²)" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4BA3AD05-1A6C-40E6-8D5A-7BDE9743BF2B}" name=" Area (KmÂ²)" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{0E49A9D5-D603-4E94-A8D7-A4BB044C0D68}" name="Migrants (net)" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{3870A96F-5DEC-436D-B51A-9A68E50275AD}" name="Fert. Rate" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{BABFD995-7631-49C4-9885-C6EA98AF96A9}" name="Med. Age"/>
-    <tableColumn id="11" xr3:uid="{0AC0476E-64A4-4044-AC9E-BFBD7D123C48}" name="Urban Pop %" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{224723EC-95FE-47F4-99C1-D101CF1E04FA}" name="World Share" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{0AC0476E-64A4-4044-AC9E-BFBD7D123C48}" name="Urban Pop %" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{224723EC-95FE-47F4-99C1-D101CF1E04FA}" name="World Share" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1719,7 +1716,7 @@
   <dimension ref="A1:L235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="K54" sqref="K54:K235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,16 +1746,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -3783,8 +3780,8 @@
       <c r="J54">
         <v>29</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>62</v>
+      <c r="K54" s="1">
+        <v>0</v>
       </c>
       <c r="L54">
         <v>0.35</v>
@@ -3795,7 +3792,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="8">
         <v>27032412</v>
@@ -3833,7 +3830,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="8">
         <v>26713205</v>
@@ -3871,7 +3868,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="8">
         <v>26498823</v>
@@ -3909,7 +3906,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="8">
         <v>24672760</v>
@@ -3947,7 +3944,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="8">
         <v>24478595</v>
@@ -3985,7 +3982,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C60" s="8">
         <v>23548781</v>
@@ -4023,7 +4020,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" s="8">
         <v>23213962</v>
@@ -4061,7 +4058,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C62" s="8">
         <v>23103565</v>
@@ -4099,7 +4096,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" s="8">
         <v>21655286</v>
@@ -4137,7 +4134,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" s="8">
         <v>21314956</v>
@@ -4175,7 +4172,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="8">
         <v>20592571</v>
@@ -4213,7 +4210,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="8">
         <v>20299123</v>
@@ -4251,7 +4248,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C67" s="8">
         <v>19764771</v>
@@ -4289,7 +4286,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C68" s="8">
         <v>19015088</v>
@@ -4327,7 +4324,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C69" s="8">
         <v>19009151</v>
@@ -4365,7 +4362,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="8">
         <v>18501984</v>
@@ -4403,7 +4400,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="8">
         <v>18406359</v>
@@ -4441,7 +4438,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C72" s="8">
         <v>18228742</v>
@@ -4479,7 +4476,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C73" s="8">
         <v>18135478</v>
@@ -4517,7 +4514,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74" s="8">
         <v>17638801</v>
@@ -4555,7 +4552,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C75" s="8">
         <v>16634373</v>
@@ -4593,7 +4590,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C76" s="8">
         <v>14754785</v>
@@ -4631,7 +4628,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C77" s="8">
         <v>14462724</v>
@@ -4669,7 +4666,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C78" s="8">
         <v>14256567</v>
@@ -4707,7 +4704,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C79" s="8">
         <v>14047786</v>
@@ -4745,7 +4742,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80" s="8">
         <v>12413315</v>
@@ -4783,7 +4780,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C81" s="8">
         <v>12277109</v>
@@ -4821,7 +4818,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C82" s="8">
         <v>11943408</v>
@@ -4859,7 +4856,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C83" s="8">
         <v>11772557</v>
@@ -4897,7 +4894,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C84" s="8">
         <v>11738763</v>
@@ -4935,7 +4932,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C85" s="8">
         <v>11552876</v>
@@ -4973,7 +4970,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C86" s="8">
         <v>11427557</v>
@@ -5011,7 +5008,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" s="8">
         <v>11027129</v>
@@ -5049,7 +5046,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88" s="8">
         <v>10979783</v>
@@ -5087,7 +5084,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C89" s="8">
         <v>10825703</v>
@@ -5125,7 +5122,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C90" s="8">
         <v>10735859</v>
@@ -5163,7 +5160,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91" s="8">
         <v>10606999</v>
@@ -5201,7 +5198,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C92" s="8">
         <v>10590927</v>
@@ -5239,7 +5236,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="8">
         <v>10576502</v>
@@ -5277,7 +5274,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C94" s="8">
         <v>10425292</v>
@@ -5315,7 +5312,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C95" s="8">
         <v>10336577</v>
@@ -5353,7 +5350,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C96" s="8">
         <v>10047817</v>
@@ -5391,7 +5388,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C97" s="8">
         <v>9676135</v>
@@ -5429,7 +5426,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C98" s="8">
         <v>9515236</v>
@@ -5467,7 +5464,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99" s="8">
         <v>9387021</v>
@@ -5505,7 +5502,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C100" s="8">
         <v>9120813</v>
@@ -5543,7 +5540,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C101" s="8">
         <v>9056696</v>
@@ -5581,7 +5578,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C102" s="8">
         <v>8921981</v>
@@ -5619,7 +5616,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C103" s="8">
         <v>8642022</v>
@@ -5657,7 +5654,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C104" s="8">
         <v>7769819</v>
@@ -5695,7 +5692,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C105" s="8">
         <v>7494498</v>
@@ -5733,7 +5730,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C106" s="8">
         <v>7414909</v>
@@ -5759,8 +5756,8 @@
       <c r="J106">
         <v>47</v>
       </c>
-      <c r="K106" s="1" t="s">
-        <v>62</v>
+      <c r="K106" s="1">
+        <v>0</v>
       </c>
       <c r="L106">
         <v>0.09</v>
@@ -5771,7 +5768,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C107" s="8">
         <v>7381023</v>
@@ -5809,7 +5806,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C108" s="8">
         <v>7186009</v>
@@ -5847,7 +5844,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C109" s="8">
         <v>6929153</v>
@@ -5885,7 +5882,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C110" s="8">
         <v>6916140</v>
@@ -5923,7 +5920,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C111" s="8">
         <v>6757689</v>
@@ -5961,7 +5958,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C112" s="8">
         <v>6736216</v>
@@ -5999,7 +5996,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C113" s="8">
         <v>6338193</v>
@@ -6037,7 +6034,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C114" s="8">
         <v>6332961</v>
@@ -6075,7 +6072,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C115" s="8">
         <v>5977412</v>
@@ -6113,7 +6110,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C116" s="8">
         <v>5832387</v>
@@ -6139,8 +6136,8 @@
       <c r="J116">
         <v>36</v>
       </c>
-      <c r="K116" s="1" t="s">
-        <v>62</v>
+      <c r="K116" s="1">
+        <v>0</v>
       </c>
       <c r="L116">
         <v>7.0000000000000007E-2</v>
@@ -6151,7 +6148,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C117" s="8">
         <v>5805962</v>
@@ -6189,7 +6186,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C118" s="8">
         <v>5617310</v>
@@ -6227,7 +6224,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C119" s="8">
         <v>5612817</v>
@@ -6265,7 +6262,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C120" s="8">
         <v>5576660</v>
@@ -6303,7 +6300,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C121" s="8">
         <v>5506760</v>
@@ -6341,7 +6338,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C122" s="8">
         <v>5495443</v>
@@ -6379,7 +6376,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C123" s="8">
         <v>5330690</v>
@@ -6417,7 +6414,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C124" s="8">
         <v>5281538</v>
@@ -6455,7 +6452,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C125" s="8">
         <v>5255017</v>
@@ -6493,7 +6490,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C126" s="8">
         <v>5213944</v>
@@ -6531,7 +6528,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C127" s="8">
         <v>5169395</v>
@@ -6569,7 +6566,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C128" s="8">
         <v>5129910</v>
@@ -6607,7 +6604,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C129" s="8">
         <v>4934507</v>
@@ -6645,7 +6642,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C130" s="8">
         <v>4515577</v>
@@ -6683,7 +6680,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C131" s="8">
         <v>3875325</v>
@@ -6721,7 +6718,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C132" s="8">
         <v>3807670</v>
@@ -6759,7 +6756,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C133" s="8">
         <v>3535603</v>
@@ -6797,7 +6794,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C134" s="8">
         <v>3475540</v>
@@ -6835,7 +6832,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C135" s="8">
         <v>3386588</v>
@@ -6861,8 +6858,8 @@
       <c r="J135">
         <v>36</v>
       </c>
-      <c r="K135" s="1" t="s">
-        <v>62</v>
+      <c r="K135" s="1">
+        <v>0</v>
       </c>
       <c r="L135">
         <v>0.04</v>
@@ -6873,7 +6870,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C136" s="8">
         <v>3242204</v>
@@ -6899,8 +6896,8 @@
       <c r="J136">
         <v>45</v>
       </c>
-      <c r="K136" s="1" t="s">
-        <v>62</v>
+      <c r="K136" s="1">
+        <v>0</v>
       </c>
       <c r="L136">
         <v>0.04</v>
@@ -6911,7 +6908,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C137" s="8">
         <v>3164253</v>
@@ -6949,7 +6946,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C138" s="8">
         <v>3048423</v>
@@ -6987,7 +6984,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C139" s="8">
         <v>3034961</v>
@@ -7025,7 +7022,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C140" s="8">
         <v>3030131</v>
@@ -7063,7 +7060,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C141" s="8">
         <v>2973840</v>
@@ -7101,7 +7098,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C142" s="8">
         <v>2859110</v>
@@ -7139,7 +7136,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C143" s="8">
         <v>2839175</v>
@@ -7177,7 +7174,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C144" s="8">
         <v>2791765</v>
@@ -7215,7 +7212,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C145" s="8">
         <v>2759988</v>
@@ -7253,7 +7250,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C146" s="8">
         <v>2538952</v>
@@ -7291,7 +7288,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C147" s="8">
         <v>2521139</v>
@@ -7329,7 +7326,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C148" s="8">
         <v>2337423</v>
@@ -7367,7 +7364,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C149" s="8">
         <v>2201352</v>
@@ -7405,7 +7402,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C150" s="8">
         <v>2118697</v>
@@ -7443,7 +7440,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C151" s="8">
         <v>1892516</v>
@@ -7481,7 +7478,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C152" s="8">
         <v>1871871</v>
@@ -7519,7 +7516,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C153" s="8">
         <v>1823009</v>
@@ -7557,7 +7554,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C154" s="8">
         <v>1607049</v>
@@ -7583,8 +7580,8 @@
       <c r="J154">
         <v>33</v>
       </c>
-      <c r="K154" s="1" t="s">
-        <v>62</v>
+      <c r="K154" s="1">
+        <v>0</v>
       </c>
       <c r="L154">
         <v>0.02</v>
@@ -7595,7 +7592,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C155" s="8">
         <v>1507782</v>
@@ -7633,7 +7630,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C156" s="8">
         <v>1400638</v>
@@ -7671,7 +7668,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C157" s="8">
         <v>1360546</v>
@@ -7709,7 +7706,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C158" s="8">
         <v>1358282</v>
@@ -7747,7 +7744,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C159" s="8">
         <v>1271169</v>
@@ -7785,7 +7782,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C160" s="8">
         <v>1242822</v>
@@ -7823,7 +7820,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C161" s="8">
         <v>1168722</v>
@@ -7861,7 +7858,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C162" s="8">
         <v>928784</v>
@@ -7899,7 +7896,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C163" s="8">
         <v>878591</v>
@@ -7925,8 +7922,8 @@
       <c r="J163">
         <v>38</v>
       </c>
-      <c r="K163" s="1" t="s">
-        <v>62</v>
+      <c r="K163" s="1">
+        <v>0</v>
       </c>
       <c r="L163">
         <v>0.01</v>
@@ -7937,7 +7934,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C164" s="8">
         <v>866628</v>
@@ -7975,7 +7972,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C165" s="8">
         <v>831087</v>
@@ -8013,7 +8010,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C166" s="8">
         <v>819198</v>
@@ -8051,7 +8048,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C167" s="8">
         <v>791524</v>
@@ -8089,7 +8086,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C168" s="8">
         <v>720262</v>
@@ -8127,7 +8124,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C169" s="8">
         <v>673036</v>
@@ -8165,7 +8162,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C170" s="8">
         <v>638479</v>
@@ -8203,7 +8200,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C171" s="8">
         <v>634431</v>
@@ -8241,7 +8238,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C172" s="8">
         <v>590506</v>
@@ -8279,7 +8276,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C173" s="8">
         <v>539607</v>
@@ -8317,7 +8314,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C174" s="8">
         <v>527799</v>
@@ -8355,7 +8352,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C175" s="8">
         <v>526923</v>
@@ -8393,7 +8390,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C176" s="8">
         <v>524877</v>
@@ -8431,7 +8428,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C177" s="8">
         <v>462721</v>
@@ -8469,7 +8466,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C178" s="8">
         <v>417072</v>
@@ -8507,7 +8504,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C179" s="8">
         <v>401283</v>
@@ -8545,7 +8542,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C180" s="8">
         <v>393396</v>
@@ -8583,7 +8580,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C181" s="8">
         <v>375106</v>
@@ -8609,8 +8606,8 @@
       <c r="J181">
         <v>47</v>
       </c>
-      <c r="K181" s="1" t="s">
-        <v>62</v>
+      <c r="K181" s="1">
+        <v>0</v>
       </c>
       <c r="L181">
         <v>0</v>
@@ -8621,7 +8618,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C182" s="8">
         <v>343195</v>
@@ -8647,8 +8644,8 @@
       <c r="J182">
         <v>49</v>
       </c>
-      <c r="K182" s="1" t="s">
-        <v>62</v>
+      <c r="K182" s="1">
+        <v>0</v>
       </c>
       <c r="L182">
         <v>0</v>
@@ -8659,7 +8656,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C183" s="8">
         <v>327777</v>
@@ -8697,7 +8694,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C184" s="8">
         <v>326505</v>
@@ -8735,7 +8732,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C185" s="8">
         <v>308522</v>
@@ -8773,7 +8770,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C186" s="8">
         <v>292639</v>
@@ -8811,7 +8808,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C187" s="8">
         <v>282467</v>
@@ -8849,7 +8846,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C188" s="8">
         <v>281807</v>
@@ -8887,7 +8884,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C189" s="8">
         <v>235536</v>
@@ -8925,7 +8922,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C190" s="8">
         <v>218019</v>
@@ -8963,7 +8960,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C191" s="8">
         <v>185482</v>
@@ -9001,7 +8998,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C192" s="8">
         <v>179744</v>
@@ -9039,7 +9036,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C193" s="8">
         <v>167777</v>
@@ -9077,7 +9074,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C194" s="8">
         <v>134518</v>
@@ -9115,7 +9112,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C195" s="8">
         <v>130418</v>
@@ -9153,7 +9150,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C196" s="8">
         <v>117207</v>
@@ -9191,7 +9188,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C197" s="8">
         <v>108066</v>
@@ -9229,7 +9226,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C198" s="8">
         <v>104175</v>
@@ -9267,7 +9264,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C199" s="8">
         <v>100616</v>
@@ -9305,7 +9302,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C200" s="8">
         <v>93772</v>
@@ -9343,7 +9340,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C201" s="8">
         <v>84905</v>
@@ -9369,8 +9366,8 @@
       <c r="J201">
         <v>45</v>
       </c>
-      <c r="K201" s="1" t="s">
-        <v>62</v>
+      <c r="K201" s="1">
+        <v>0</v>
       </c>
       <c r="L201">
         <v>0</v>
@@ -9381,7 +9378,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C202" s="8">
         <v>8416</v>
@@ -9419,7 +9416,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C203" s="8">
         <v>81938</v>
@@ -9457,7 +9454,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C204" s="8">
         <v>74457</v>
@@ -9495,7 +9492,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C205" s="8">
         <v>66205</v>
@@ -9533,7 +9530,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C206" s="8">
         <v>64636</v>
@@ -9571,7 +9568,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C207" s="8">
         <v>5584</v>
@@ -9609,7 +9606,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C208" s="8">
         <v>554</v>
@@ -9647,7 +9644,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C209" s="8">
         <v>46843</v>
@@ -9685,7 +9682,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C210" s="8">
         <v>46765</v>
@@ -9711,8 +9708,8 @@
       <c r="J210">
         <v>29</v>
       </c>
-      <c r="K210" s="1" t="s">
-        <v>62</v>
+      <c r="K210" s="1">
+        <v>0</v>
       </c>
       <c r="L210">
         <v>0</v>
@@ -9723,7 +9720,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C211" s="8">
         <v>46535</v>
@@ -9761,7 +9758,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C212" s="8">
         <v>44278</v>
@@ -9787,8 +9784,8 @@
       <c r="J212">
         <v>37</v>
       </c>
-      <c r="K212" s="1" t="s">
-        <v>62</v>
+      <c r="K212" s="1">
+        <v>0</v>
       </c>
       <c r="L212">
         <v>0</v>
@@ -9799,7 +9796,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C213" s="8">
         <v>4335</v>
@@ -9837,7 +9834,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C214" s="8">
         <v>3987</v>
@@ -9875,7 +9872,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C215" s="8">
         <v>39471</v>
@@ -9913,7 +9910,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C216" s="8">
         <v>39329</v>
@@ -9951,7 +9948,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C217" s="8">
         <v>38631</v>
@@ -9977,8 +9974,8 @@
       <c r="J217">
         <v>54</v>
       </c>
-      <c r="K217" s="1" t="s">
-        <v>62</v>
+      <c r="K217" s="1">
+        <v>0</v>
       </c>
       <c r="L217">
         <v>0</v>
@@ -9989,7 +9986,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C218" s="8">
         <v>37548</v>
@@ -10015,8 +10012,8 @@
       <c r="J218">
         <v>21</v>
       </c>
-      <c r="K218" s="1" t="s">
-        <v>62</v>
+      <c r="K218" s="1">
+        <v>0</v>
       </c>
       <c r="L218">
         <v>0</v>
@@ -10027,7 +10024,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C219" s="8">
         <v>33581</v>
@@ -10065,7 +10062,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C220" s="8">
         <v>30675</v>
@@ -10103,7 +10100,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C221" s="8">
         <v>26129</v>
@@ -10141,7 +10138,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C222" s="8">
         <v>17695</v>
@@ -10167,8 +10164,8 @@
       <c r="J222">
         <v>38</v>
       </c>
-      <c r="K222" s="1" t="s">
-        <v>62</v>
+      <c r="K222" s="1">
+        <v>0</v>
       </c>
       <c r="L222">
         <v>0</v>
@@ -10179,7 +10176,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C223" s="8">
         <v>14598</v>
@@ -10205,8 +10202,8 @@
       <c r="J223">
         <v>38</v>
       </c>
-      <c r="K223" s="1" t="s">
-        <v>62</v>
+      <c r="K223" s="1">
+        <v>0</v>
       </c>
       <c r="L223">
         <v>0</v>
@@ -10217,7 +10214,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C224" s="8">
         <v>13729</v>
@@ -10255,7 +10252,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C225" s="8">
         <v>11947</v>
@@ -10293,7 +10290,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C226" s="8">
         <v>11277</v>
@@ -10331,7 +10328,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C227" s="8">
         <v>11258</v>
@@ -10369,7 +10366,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C228" s="8">
         <v>9646</v>
@@ -10407,7 +10404,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C229" s="8">
         <v>5628</v>
@@ -10433,8 +10430,8 @@
       <c r="J229">
         <v>47</v>
       </c>
-      <c r="K229" s="1" t="s">
-        <v>62</v>
+      <c r="K229" s="1">
+        <v>0</v>
       </c>
       <c r="L229">
         <v>0</v>
@@ -10445,7 +10442,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C230" s="8">
         <v>5237</v>
@@ -10483,7 +10480,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C231" s="8">
         <v>4389</v>
@@ -10521,7 +10518,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C232" s="8">
         <v>347</v>
@@ -10559,7 +10556,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C233" s="8">
         <v>2506</v>
@@ -10597,7 +10594,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C234" s="8">
         <v>1819</v>
@@ -10635,7 +10632,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C235" s="8">
         <v>496</v>
@@ -10661,8 +10658,8 @@
       <c r="J235">
         <v>59</v>
       </c>
-      <c r="K235" s="1" t="s">
-        <v>62</v>
+      <c r="K235" s="1">
+        <v>0</v>
       </c>
       <c r="L235">
         <v>0</v>

</xml_diff>

<commit_message>
Inclusão de tabela continent
A inclusão da tabela no arquivo de excel se faz necessario para correlacionar pais + continente
</commit_message>
<xml_diff>
--- a/Wolrd Population Data.xlsx
+++ b/Wolrd Population Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263d74c401730189/Desktop/Wold/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{7AC64A1E-81AA-459C-B91C-A743A76CC10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0038BDB3-9593-4042-8CE1-0D6D65EE391B}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{7AC64A1E-81AA-459C-B91C-A743A76CC10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA2F855-6FFE-4BE6-8C2B-00509C54EBC2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A9A4517-54CC-463D-B5FC-53C5F03393D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1A9A4517-54CC-463D-B5FC-53C5F03393D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Wolrd Population Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Continentes " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="262">
   <si>
     <t>Rank</t>
   </si>
@@ -771,6 +772,54 @@
   </si>
   <si>
     <t xml:space="preserve"> Area (KmÂ²)</t>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Vatican City</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>South America</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1213,6 +1262,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1259,7 +1321,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1281,6 +1343,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1327,7 +1393,50 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1379,18 +1488,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E40C16B-B3E3-457F-B36F-12DDA6F5217B}" name="Wolrd_Population_Data" displayName="Wolrd_Population_Data" ref="A1:L235" totalsRowShown="0">
   <autoFilter ref="A1:L235" xr:uid="{1E40C16B-B3E3-457F-B36F-12DDA6F5217B}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{10E32209-646A-4AEE-AB9D-114FED796C19}" name="Rank" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A7480106-A65C-48C7-84E9-060389FC7134}" name="Country" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4EC52585-D6F6-4D64-B4E4-399D26A08785}" name="Population (2024)" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{10E32209-646A-4AEE-AB9D-114FED796C19}" name="Rank" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A7480106-A65C-48C7-84E9-060389FC7134}" name="Country" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{4EC52585-D6F6-4D64-B4E4-399D26A08785}" name="Population (2024)" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{F0290345-2A39-431A-8F0F-7B2DFC7127B0}" name="Mudanca_Anual" dataCellStyle="Porcentagem"/>
-    <tableColumn id="5" xr3:uid="{4CC63AA6-A78C-42B8-85A4-140D8A90862B}" name="Mudanca_Liquida" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F48D8035-F4B0-4B4D-8A5A-AEA88F7EFD59}" name="Density (P/KmÂ²)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4BA3AD05-1A6C-40E6-8D5A-7BDE9743BF2B}" name=" Area (KmÂ²)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{0E49A9D5-D603-4E94-A8D7-A4BB044C0D68}" name="Migrants (net)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{3870A96F-5DEC-436D-B51A-9A68E50275AD}" name="Fert. Rate" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{4CC63AA6-A78C-42B8-85A4-140D8A90862B}" name="Mudanca_Liquida" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{F48D8035-F4B0-4B4D-8A5A-AEA88F7EFD59}" name="Density (P/KmÂ²)" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4BA3AD05-1A6C-40E6-8D5A-7BDE9743BF2B}" name=" Area (KmÂ²)" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{0E49A9D5-D603-4E94-A8D7-A4BB044C0D68}" name="Migrants (net)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{3870A96F-5DEC-436D-B51A-9A68E50275AD}" name="Fert. Rate" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{BABFD995-7631-49C4-9885-C6EA98AF96A9}" name="Med. Age"/>
-    <tableColumn id="11" xr3:uid="{0AC0476E-64A4-4044-AC9E-BFBD7D123C48}" name="Urban Pop %" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{224723EC-95FE-47F4-99C1-D101CF1E04FA}" name="World Share" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{0AC0476E-64A4-4044-AC9E-BFBD7D123C48}" name="Urban Pop %" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{224723EC-95FE-47F4-99C1-D101CF1E04FA}" name="World Share" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{903DF17A-C50D-4566-A801-BD11C6BE348D}" name="Continent" displayName="Continent" ref="A1:B196" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:B196" xr:uid="{903DF17A-C50D-4566-A801-BD11C6BE348D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4B0FD9DF-B999-410B-A9E3-046DBFF31393}" name="Country"/>
+    <tableColumn id="2" xr3:uid="{806E9EA7-82A5-43FD-B104-3D17743EC338}" name="Continent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1715,7 +1835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE97948-A1B7-477A-A78D-F9C6C6B87574}">
   <dimension ref="A1:L235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K54" sqref="K54:K235"/>
     </sheetView>
   </sheetViews>
@@ -10672,4 +10792,1594 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F1014C-C691-4FDA-97CC-9CFB4E8718C9}">
+  <dimension ref="A1:B196"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B157" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B163" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B164" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B166" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B167" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B168" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B169" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B170" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B171" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B172" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B173" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B174" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B175" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B176" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B177" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="B178" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B179" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B180" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B181" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B182" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B183" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B185" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B186" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B187" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B188" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B189" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B190" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B191" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B192" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B193" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B194" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B195" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B196" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>